<commit_message>
rmm corrigida para 2022
</commit_message>
<xml_diff>
--- a/data-raw/extracao-dos-dados/databases-antigas/analises_obitos_RMM_1996_2021.xlsx
+++ b/data-raw/extracao-dos-dados/databases-antigas/analises_obitos_RMM_1996_2021.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive - Universidade Federal do Espírito Santo\Documentos\apainel-vigilancia-saude-materna-v2\data-raw\extracao-dos-dados\databases-antigas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2A4ECEC8F95D4C32B913461A3D45A947C445F5A8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0CC18502-DD79-46E9-9E2D-ACA077FD066A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMM_1996_2021_R_program" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -39,11 +45,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -67,7 +73,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -123,11 +129,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -141,12 +160,26 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,11 +254,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -267,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,9 +340,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,6 +392,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,16 +585,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:E27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="29">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1996</v>
       </c>
@@ -546,13 +623,13 @@
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:D26" si="0">(B2/C2)*100000</f>
-        <v>51.130142509145536</v>
+        <v>51.130142509145543</v>
       </c>
       <c r="E2" s="4">
         <v>103.21</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1997</v>
       </c>
@@ -570,7 +647,7 @@
         <v>109.66</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>1998</v>
       </c>
@@ -588,7 +665,7 @@
         <v>110.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1999</v>
       </c>
@@ -606,7 +683,7 @@
         <v>92.26</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2000</v>
       </c>
@@ -624,7 +701,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>2001</v>
       </c>
@@ -642,7 +719,7 @@
         <v>70.91</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>2002</v>
       </c>
@@ -660,7 +737,7 @@
         <v>75.87</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>2003</v>
       </c>
@@ -678,7 +755,7 @@
         <v>72.989999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2004</v>
       </c>
@@ -696,7 +773,7 @@
         <v>76.09</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>2005</v>
       </c>
@@ -714,7 +791,7 @@
         <v>74.680000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>2006</v>
       </c>
@@ -732,7 +809,7 @@
         <v>77.16</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>2007</v>
       </c>
@@ -750,7 +827,7 @@
         <v>76.989999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>2008</v>
       </c>
@@ -768,7 +845,7 @@
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2009</v>
       </c>
@@ -786,7 +863,7 @@
         <v>72.420218701047702</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2010</v>
       </c>
@@ -804,7 +881,7 @@
         <v>68.938568645893895</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>2011</v>
       </c>
@@ -822,7 +899,7 @@
         <v>61.785803332372701</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>2012</v>
       </c>
@@ -840,7 +917,7 @@
         <v>59.327857704478603</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>2013</v>
       </c>
@@ -858,7 +935,7 @@
         <v>62.088184334636303</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>2014</v>
       </c>
@@ -876,7 +953,7 @@
         <v>63.786628691251501</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>2015</v>
       </c>
@@ -894,7 +971,7 @@
         <v>62.018613384378</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>2016</v>
       </c>
@@ -912,7 +989,7 @@
         <v>64.420183357827696</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>2017</v>
       </c>
@@ -930,7 +1007,7 @@
         <v>64.510943087734603</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>2018</v>
       </c>
@@ -948,7 +1025,7 @@
         <v>59.116475354948797</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>2019</v>
       </c>
@@ -966,7 +1043,7 @@
         <v>57.930025347946398</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>2020</v>
       </c>
@@ -984,22 +1061,33 @@
         <v>74.6937983147415</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>2021</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="7">
         <v>3025</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="8">
         <v>2677101</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="9">
         <f>(B27/C27)*100000</f>
         <v>112.99536326795291</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>117.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="11">
+        <v>57.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>